<commit_message>
Final Changes for PRJ0018286-CF Industry Group Changes TECH
</commit_message>
<xml_diff>
--- a/TestData/TMTI0046471_VerifyCompaniesHasNestedListToShowHLRelationshipForContacts.xlsx
+++ b/TestData/TMTI0046471_VerifyCompaniesHasNestedListToShowHLRelationshipForContacts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay.kumar\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VKumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43E9F49-4957-47A8-96CB-BFD19FB80306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0F3E1D-05B3-44CA-ADFA-551071C9D78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{D381DC3E-0C7A-48CF-8E3B-36CB765DCADA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14640" activeTab="4" xr2:uid="{D381DC3E-0C7A-48CF-8E3B-36CB765DCADA}"/>
   </bookViews>
   <sheets>
     <sheet name="Companies" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>StdUser</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Relationships</t>
+  </si>
+  <si>
+    <t>Adam Cole</t>
   </si>
 </sst>
 </file>
@@ -464,22 +467,22 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -493,7 +496,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -503,7 +506,7 @@
       <c r="D2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -526,17 +529,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -554,17 +557,17 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -582,19 +585,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -608,19 +611,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4922F08E-3E13-47AA-BD27-63BC12B6D061}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -632,19 +635,21 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
     </row>
   </sheetData>
@@ -656,26 +661,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5D965E-88C7-439C-916A-F788D109B4B4}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>

</xml_diff>